<commit_message>
added homogenized channel method - can now homogenize many channels into a single channel
</commit_message>
<xml_diff>
--- a/Data/msre_flow_setup.xlsx
+++ b/Data/msre_flow_setup.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\jonathon\projects\mothman\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\moosetools\projects\mothman\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{404E139A-34F8-4141-B2E2-DA1F46160F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F019C9-8FB6-4F45-93C8-AB2A07D50174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{553CB2C9-4EE1-4D00-87D2-592D4CC4367C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{553CB2C9-4EE1-4D00-87D2-592D4CC4367C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="8channel model" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>Time</t>
   </si>
@@ -185,6 +185,42 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Channel Set</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Scalars</t>
+  </si>
+  <si>
+    <t>F_total</t>
+  </si>
+  <si>
+    <t>F*V</t>
+  </si>
+  <si>
+    <t>F*V_norm'd</t>
+  </si>
+  <si>
+    <t>Area m2</t>
+  </si>
+  <si>
+    <t>Density 900K</t>
+  </si>
+  <si>
+    <t>area full</t>
+  </si>
+  <si>
+    <t>Density kg/m3 900K</t>
+  </si>
+  <si>
+    <t>Mdot kg/s</t>
   </si>
 </sst>
 </file>
@@ -196,7 +232,7 @@
     <numFmt numFmtId="165" formatCode="0.000000000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +265,26 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF79FFD7"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFCA74C"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -256,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,6 +324,15 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D096EF0A-A8F7-4824-A408-62772B98A0D8}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,4 +1469,328 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2DF1A60-BD23-43FA-8C61-A780C983F3DF}">
+  <dimension ref="A2:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>4.1445591888752196</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3" s="10">
+        <v>1.13132731957521E-8</v>
+      </c>
+      <c r="E3" s="11" cm="1">
+        <f t="array" ref="E3:E10">D3:D10/B21</f>
+        <v>1.9056945196436689E-2</v>
+      </c>
+      <c r="F3">
+        <f>67*2.54/100</f>
+        <v>1.7018</v>
+      </c>
+      <c r="G3">
+        <f>$B$22</f>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H3">
+        <f>$B$24</f>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>7.8013296890102204</v>
+      </c>
+      <c r="C4">
+        <v>36</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2.7728540558819001E-8</v>
+      </c>
+      <c r="E4" s="11">
+        <v>4.6708080735201989E-2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F10" si="0">67*2.54/100</f>
+        <v>1.7018</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G10" si="1">$B$22</f>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H10" si="2">$B$24</f>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
+        <v>7.9938866900744001</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
+      <c r="D5" s="10">
+        <v>5.8679342783278698E-8</v>
+      </c>
+      <c r="E5" s="11">
+        <v>9.884398619523696E-2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.7018</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>8.2612147279731403</v>
+      </c>
+      <c r="C6">
+        <v>176</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1.3340196610763899E-7</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.22471250479169344</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.7018</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>8.5611534676762595</v>
+      </c>
+      <c r="C7">
+        <v>240</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1.4892733158460401E-7</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.25086462133036808</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.7018</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
+        <v>8.8340275917503899</v>
+      </c>
+      <c r="C8">
+        <v>280</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1.24890632355603E-7</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.21037536132714471</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1.7018</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9">
+        <v>9.2099026961714205</v>
+      </c>
+      <c r="C9">
+        <v>332</v>
+      </c>
+      <c r="D9" s="10">
+        <v>8.0280353584149203E-8</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0.13523038577183272</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1.7018</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9">
+        <v>12.632149904758901</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="10">
+        <v>8.4347350007422497E-9</v>
+      </c>
+      <c r="E10" s="11">
+        <v>1.4208114652085489E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1.7018</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>2.8758716236800002E-4</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="10">
+        <f>SUM(D3:D10)</f>
+        <v>5.9365617517058723E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="13">
+        <v>2.8758716236800002E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <f>2715.13-0.513*B23</f>
+        <v>2253.4300000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>